<commit_message>
[+/*] Batch unit tests added
</commit_message>
<xml_diff>
--- a/src/test/resources/file/insert_users.xlsx
+++ b/src/test/resources/file/insert_users.xlsx
@@ -24,17 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="77">
   <si>
     <t>username</t>
   </si>
   <si>
-    <t>first name</t>
-  </si>
-  <si>
-    <t>last name</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -135,6 +129,132 @@
   </si>
   <si>
     <t>username10@gmail.com</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>username11</t>
+  </si>
+  <si>
+    <t>username12</t>
+  </si>
+  <si>
+    <t>username13</t>
+  </si>
+  <si>
+    <t>username14</t>
+  </si>
+  <si>
+    <t>username15</t>
+  </si>
+  <si>
+    <t>username16</t>
+  </si>
+  <si>
+    <t>username17</t>
+  </si>
+  <si>
+    <t>username18</t>
+  </si>
+  <si>
+    <t>username19</t>
+  </si>
+  <si>
+    <t>username20</t>
+  </si>
+  <si>
+    <t>password11</t>
+  </si>
+  <si>
+    <t>password12</t>
+  </si>
+  <si>
+    <t>password13</t>
+  </si>
+  <si>
+    <t>password14</t>
+  </si>
+  <si>
+    <t>password15</t>
+  </si>
+  <si>
+    <t>password16</t>
+  </si>
+  <si>
+    <t>password17</t>
+  </si>
+  <si>
+    <t>password18</t>
+  </si>
+  <si>
+    <t>password19</t>
+  </si>
+  <si>
+    <t>password20</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>user4</t>
+  </si>
+  <si>
+    <t>user5</t>
+  </si>
+  <si>
+    <t>user6</t>
+  </si>
+  <si>
+    <t>user7</t>
+  </si>
+  <si>
+    <t>user8</t>
+  </si>
+  <si>
+    <t>user9</t>
+  </si>
+  <si>
+    <t>user10</t>
+  </si>
+  <si>
+    <t>user11</t>
+  </si>
+  <si>
+    <t>user12</t>
+  </si>
+  <si>
+    <t>user13</t>
+  </si>
+  <si>
+    <t>user14</t>
+  </si>
+  <si>
+    <t>user15</t>
+  </si>
+  <si>
+    <t>user16</t>
+  </si>
+  <si>
+    <t>user17</t>
+  </si>
+  <si>
+    <t>user18</t>
+  </si>
+  <si>
+    <t>user19</t>
+  </si>
+  <si>
+    <t>user20</t>
   </si>
 </sst>
 </file>
@@ -465,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -485,39 +605,39 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -528,19 +648,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -551,19 +671,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -574,19 +694,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -597,19 +717,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -620,19 +740,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -643,19 +763,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
@@ -666,19 +786,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -689,19 +809,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
@@ -712,25 +832,255 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" t="b">
-        <v>1</v>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -745,8 +1095,18 @@
     <hyperlink ref="E9" r:id="rId8"/>
     <hyperlink ref="E7" r:id="rId9"/>
     <hyperlink ref="E10" r:id="rId10"/>
+    <hyperlink ref="E12" r:id="rId11"/>
+    <hyperlink ref="E13" r:id="rId12"/>
+    <hyperlink ref="E14" r:id="rId13"/>
+    <hyperlink ref="E15" r:id="rId14"/>
+    <hyperlink ref="E18" r:id="rId15"/>
+    <hyperlink ref="E21" r:id="rId16"/>
+    <hyperlink ref="E16" r:id="rId17"/>
+    <hyperlink ref="E19" r:id="rId18"/>
+    <hyperlink ref="E17" r:id="rId19"/>
+    <hyperlink ref="E20" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>